<commit_message>
change file excel and add new txt file
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+  <si>
+    <t>asfasf</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +339,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>